<commit_message>
Many minor bug fixes
</commit_message>
<xml_diff>
--- a/inst/extdata/sNdR_sample_example_elaborate.xlsx
+++ b/inst/extdata/sNdR_sample_example_elaborate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://aarhusuniversitet-my.sharepoint.com/personal/au530301_uni_au_dk/Documents/Vedhæftede filer/THJ LAB/Projects/seqNdisplayR/seqNdisplayR/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{9140B3AB-2FC2-8B48-8275-FF91E025383F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="11_CD1A440ACD95BDEDF0F75F572355843E7E3D75CE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A05C93AB-AE5A-4E4F-9433-876A79F57C82}"/>
   <bookViews>
-    <workbookView xWindow="-9740" yWindow="-28300" windowWidth="37600" windowHeight="17040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1500" yWindow="1540" windowWidth="25560" windowHeight="18720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SAMPLES" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="214">
   <si>
     <t>color</t>
   </si>
@@ -313,27 +313,21 @@
     <t>mean</t>
   </si>
   <si>
+    <t>TRUE</t>
+  </si>
+  <si>
     <t>FALSE</t>
   </si>
   <si>
     <t>1</t>
   </si>
   <si>
-    <t>1,2,3,1,2,3,1,3,1,3,1,2,3,1,2,3,1,3,1,3</t>
-  </si>
-  <si>
     <t>NULL</t>
   </si>
   <si>
-    <t>TRUE</t>
-  </si>
-  <si>
     <t>NA,NA</t>
   </si>
   <si>
-    <t>1,2,2,2</t>
-  </si>
-  <si>
     <t>annotation_name</t>
   </si>
   <si>
@@ -658,7 +652,7 @@
     <t>track_height_cm</t>
   </si>
   <si>
-    <t>0.4</t>
+    <t>0.3</t>
   </si>
   <si>
     <t>track_width_cm</t>
@@ -703,7 +697,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <fgColor theme="2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -720,16 +714,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1037,9 +1028,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:I1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1975,9 +1964,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1987,17 +1976,16 @@
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="31.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -2017,119 +2005,110 @@
         <v>87</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>4</v>
+        <v>88</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="N1" s="2" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>13</v>
       </c>
       <c r="B2" t="s">
         <v>95</v>
       </c>
-      <c r="C2" s="3" t="b">
-        <v>1</v>
+      <c r="C2" t="s">
+        <v>96</v>
       </c>
       <c r="D2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="G2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="I2" t="s">
         <v>96</v>
       </c>
       <c r="J2" t="s">
+        <v>97</v>
+      </c>
+      <c r="K2" t="s">
         <v>100</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>96</v>
       </c>
-      <c r="L2" t="s">
-        <v>101</v>
-      </c>
       <c r="M2" t="s">
-        <v>100</v>
-      </c>
-      <c r="N2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>80</v>
       </c>
       <c r="B3" t="s">
         <v>95</v>
       </c>
-      <c r="C3" s="3" t="b">
-        <v>1</v>
+      <c r="C3" t="s">
+        <v>96</v>
       </c>
       <c r="D3" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F3" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="G3" t="s">
         <v>99</v>
       </c>
       <c r="H3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="I3" t="s">
         <v>96</v>
       </c>
       <c r="J3" t="s">
+        <v>97</v>
+      </c>
+      <c r="K3" t="s">
         <v>100</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>96</v>
       </c>
-      <c r="L3" t="s">
-        <v>101</v>
-      </c>
       <c r="M3" t="s">
-        <v>100</v>
-      </c>
-      <c r="N3" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>69</v>
       </c>
@@ -2137,43 +2116,40 @@
         <v>95</v>
       </c>
       <c r="C4" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D4" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E4" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F4" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="G4" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="H4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="I4" t="s">
         <v>96</v>
       </c>
       <c r="J4" t="s">
+        <v>97</v>
+      </c>
+      <c r="K4" t="s">
         <v>100</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>96</v>
       </c>
-      <c r="L4" t="s">
-        <v>101</v>
-      </c>
       <c r="M4" t="s">
-        <v>100</v>
-      </c>
-      <c r="N4" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>59</v>
       </c>
@@ -2181,39 +2157,36 @@
         <v>95</v>
       </c>
       <c r="C5" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D5" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E5" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F5" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="G5" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="H5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="I5" t="s">
         <v>96</v>
       </c>
       <c r="J5" t="s">
+        <v>97</v>
+      </c>
+      <c r="K5" t="s">
         <v>100</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>96</v>
       </c>
-      <c r="L5" t="s">
-        <v>101</v>
-      </c>
       <c r="M5" t="s">
-        <v>100</v>
-      </c>
-      <c r="N5" t="s">
         <v>99</v>
       </c>
     </row>
@@ -2226,9 +2199,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:H1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2243,77 +2214,77 @@
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>108</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F2" t="s">
+        <v>97</v>
+      </c>
+      <c r="G2" t="s">
         <v>111</v>
       </c>
-      <c r="B2" t="s">
+      <c r="H2" t="s">
         <v>112</v>
-      </c>
-      <c r="C2" t="s">
-        <v>100</v>
-      </c>
-      <c r="D2" t="s">
-        <v>96</v>
-      </c>
-      <c r="E2" t="s">
-        <v>96</v>
-      </c>
-      <c r="F2" t="s">
-        <v>96</v>
-      </c>
-      <c r="G2" t="s">
-        <v>113</v>
-      </c>
-      <c r="H2" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E3" t="s">
+        <v>97</v>
+      </c>
+      <c r="F3" t="s">
+        <v>97</v>
+      </c>
+      <c r="G3" t="s">
         <v>115</v>
-      </c>
-      <c r="B3" t="s">
-        <v>116</v>
-      </c>
-      <c r="C3" t="s">
-        <v>100</v>
-      </c>
-      <c r="D3" t="s">
-        <v>96</v>
-      </c>
-      <c r="E3" t="s">
-        <v>96</v>
-      </c>
-      <c r="F3" t="s">
-        <v>96</v>
-      </c>
-      <c r="G3" t="s">
-        <v>117</v>
       </c>
       <c r="H3" t="s">
         <v>99</v>
@@ -2321,28 +2292,28 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C4" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D4" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E4" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F4" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="G4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="H4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -2354,9 +2325,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B71"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2366,31 +2335,31 @@
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B2" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B4" t="s">
         <v>99</v>
@@ -2398,39 +2367,39 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B6" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B7" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B8" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B9" t="s">
         <v>99</v>
@@ -2438,63 +2407,63 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B10" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B11" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B12" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B13" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B14" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B15" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B16" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B17" t="s">
         <v>99</v>
@@ -2502,26 +2471,26 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B18" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B19" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B20" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -2534,7 +2503,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B22" t="s">
         <v>99</v>
@@ -2542,7 +2511,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B23" t="s">
         <v>99</v>
@@ -2550,15 +2519,15 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B24" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B25" t="s">
         <v>99</v>
@@ -2566,23 +2535,23 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B26" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B27" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B28" t="s">
         <v>99</v>
@@ -2590,15 +2559,15 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B29" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B30" t="s">
         <v>99</v>
@@ -2606,87 +2575,87 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B31" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B32" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B33" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B34" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B35" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B36" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B37" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B38" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B39" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B40" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B41" t="s">
         <v>99</v>
@@ -2694,7 +2663,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B42" t="s">
         <v>99</v>
@@ -2702,39 +2671,39 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B43" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B44" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B45" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B46" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B47" t="s">
         <v>99</v>
@@ -2742,7 +2711,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B48" t="s">
         <v>99</v>
@@ -2750,7 +2719,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B49" t="s">
         <v>99</v>
@@ -2758,7 +2727,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B50" t="s">
         <v>99</v>
@@ -2766,7 +2735,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B51" t="s">
         <v>99</v>
@@ -2774,15 +2743,15 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B52" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B53" t="s">
         <v>99</v>
@@ -2790,7 +2759,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B54" t="s">
         <v>99</v>
@@ -2798,23 +2767,23 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B55" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B56" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B57" t="s">
         <v>99</v>
@@ -2822,47 +2791,47 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B58" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B59" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B60" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B61" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B62" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B63" t="s">
         <v>99</v>
@@ -2870,66 +2839,66 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B64" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B65" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B66" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B67" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B68" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B69" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B70" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B71" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
   </sheetData>

</xml_diff>